<commit_message>
connected letter system to visualization
</commit_message>
<xml_diff>
--- a/MiningPrototype/Assets/Other/Letters.xlsx
+++ b/MiningPrototype/Assets/Other/Letters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\BAMiningPrototype\MiningPrototype\Assets\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78F8094-A67E-4ABF-A30A-5729FAD9DA0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0837F5B-E8F1-43AF-BCE3-8DDCE2FA4707}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7650" yWindow="990" windowWidth="16380" windowHeight="13635" xr2:uid="{0D810164-3444-44BA-AD29-1EAC595712B8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0D810164-3444-44BA-AD29-1EAC595712B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
   <si>
     <t>Id</t>
   </si>
@@ -60,18 +60,118 @@
   <si>
     <t>Wife</t>
   </si>
+  <si>
+    <t>My beloved _____,
+I knew the journy would be a long one, but I believed that by now I would have heard back from you. Maybe by the time you receive this letter your response will have already found its way back to me. I hope the land under the cottage is as blessed as you believed.
+The nights keep getting longer, yet i don't get more sleep.
+Please come back soon so i can sleep with you again.
+With love,
+_______</t>
+  </si>
+  <si>
+    <t>Grief 1
+Shock and Denial</t>
+  </si>
+  <si>
+    <t>Grief 2
+Pain and Guild</t>
+  </si>
+  <si>
+    <t>Grief 3
+Anger and bargaining</t>
+  </si>
+  <si>
+    <t>Grief 4
+Depression</t>
+  </si>
+  <si>
+    <t>Grief 5
+Upward turn.</t>
+  </si>
+  <si>
+    <t>Grief 6
+Reconstruction</t>
+  </si>
+  <si>
+    <t>Grief 7
+Acceptance
+END</t>
+  </si>
+  <si>
+    <t>too late im out</t>
+  </si>
+  <si>
+    <t>stop sending letters to me</t>
+  </si>
+  <si>
+    <t>i've moved foreward
+I want you out of my life
+I will not respond</t>
+  </si>
+  <si>
+    <t>goodbye.</t>
+  </si>
+  <si>
+    <t>Upset Raging
+Vengeful</t>
+  </si>
+  <si>
+    <t>anger
+disappointment
+fear</t>
+  </si>
+  <si>
+    <t>Forgiving</t>
+  </si>
+  <si>
+    <t>happiness
+relieved
+curiosity</t>
+  </si>
+  <si>
+    <t>Excited, Hopeful</t>
+  </si>
+  <si>
+    <t>Loving Caring</t>
+  </si>
+  <si>
+    <t>Melancholic
+Impatient</t>
+  </si>
+  <si>
+    <t>Troubled
+Helpless</t>
+  </si>
+  <si>
+    <t>No future</t>
+  </si>
+  <si>
+    <t>I've met someone else</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1A1A1A"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1A1A1A"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -94,12 +194,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,15 +521,17 @@
   <dimension ref="A1:E248"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="38.5703125" customWidth="1"/>
-    <col min="4" max="4" width="37" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="5" width="99.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -452,165 +558,399 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="C2">
+        <v>116</v>
+      </c>
+      <c r="D2">
+        <v>101</v>
+      </c>
       <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>101</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>116</v>
+      </c>
+      <c r="D3">
+        <v>102</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>102</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>116</v>
+      </c>
+      <c r="D4">
+        <v>103</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>103</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>114</v>
+      </c>
+      <c r="D5">
+        <v>104</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>104</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>114</v>
+      </c>
+      <c r="D6">
+        <v>105</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>105</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>114</v>
+      </c>
+      <c r="D7">
+        <v>106</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>106</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>109</v>
+      </c>
+      <c r="D8">
+        <v>107</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>107</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>109</v>
+      </c>
+      <c r="D9">
+        <v>108</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>108</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>109</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>109</v>
       </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>110</v>
+      </c>
+      <c r="D11">
+        <v>112</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>110</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>111</v>
+      </c>
+      <c r="D12">
+        <v>112</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>111</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>112</v>
+      </c>
+      <c r="D13">
+        <v>112</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>112</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>113</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>110</v>
+      </c>
+      <c r="D15">
+        <v>112</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>114</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>115</v>
+      </c>
+      <c r="D16">
+        <v>113</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>115</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>117</v>
+      </c>
+      <c r="D17">
+        <v>120</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>116</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>117</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>117</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>118</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>118</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>119</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>119</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21">
+        <v>120</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>120</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22">
+        <v>121</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>121</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23">
+        <v>122</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>122</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24">
+        <v>109</v>
+      </c>
+      <c r="D24">
+        <v>112</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>126</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>128</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>129</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>130</v>
       </c>

</xml_diff>

<commit_message>
Corrected Deer to Dear in first Letter
</commit_message>
<xml_diff>
--- a/MiningPrototype/Assets/Other/Letters.xlsx
+++ b/MiningPrototype/Assets/Other/Letters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\BAMiningPrototype\MiningPrototype\Assets\Other\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\projects\01_Repositorys\BAMiningPrototype\MiningPrototype\Assets\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89516549-F8B3-4352-BA68-F5C5669AD7AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF68CF7-48EC-47CC-8182-74401805433A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0D810164-3444-44BA-AD29-1EAC595712B8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{0D810164-3444-44BA-AD29-1EAC595712B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,14 +47,6 @@
     <t>Ignore</t>
   </si>
   <si>
-    <t>Deer ____,
-by the time you will read this letter, we will have parted for many moons. For me, you just left a few days ago. I've organized the delivery of some basic necessities as we had discussed. Hopefully, they will be waiting for you at the cottage. The old mans house is not nothing spectacular, but it should keep you warm in your endevour.
-My nights have been filled with horror. I dream that you never arrive. I dream that you will never return.
- But as we decided I will wait for you.
-Yours truly,
-______</t>
-  </si>
-  <si>
     <t>Author</t>
   </si>
   <si>
@@ -147,6 +139,14 @@
   </si>
   <si>
     <t>I've met someone else</t>
+  </si>
+  <si>
+    <t>Dear ____,
+by the time you will read this letter, we will have parted for many moons. For me, you just left a few days ago. I've organized the delivery of some basic necessities as we had discussed. Hopefully, they will be waiting for you at the cottage. The old mans house is not nothing spectacular, but it should keep you warm in your endevour.
+My nights have been filled with horror. I dream that you never arrive. I dream that you will never return.
+ But as we decided I will wait for you.
+Yours truly,
+______</t>
   </si>
 </sst>
 </file>
@@ -206,7 +206,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -222,7 +222,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -521,25 +521,25 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="99.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="1" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="99.88671875" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -551,12 +551,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>116</v>
@@ -565,15 +565,15 @@
         <v>101</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>116</v>
@@ -582,15 +582,15 @@
         <v>102</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>116</v>
@@ -599,15 +599,15 @@
         <v>103</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>114</v>
@@ -616,15 +616,15 @@
         <v>104</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>114</v>
@@ -633,15 +633,15 @@
         <v>105</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>105</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>114</v>
@@ -650,15 +650,15 @@
         <v>106</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>106</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>109</v>
@@ -667,15 +667,15 @@
         <v>107</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>107</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9">
         <v>109</v>
@@ -684,29 +684,29 @@
         <v>108</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>108</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <v>109</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>109</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11">
         <v>110</v>
@@ -715,15 +715,15 @@
         <v>112</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>110</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12">
         <v>111</v>
@@ -732,15 +732,15 @@
         <v>112</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>111</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13">
         <v>112</v>
@@ -749,26 +749,26 @@
         <v>112</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>112</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>113</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15">
         <v>110</v>
@@ -777,15 +777,15 @@
         <v>112</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>114</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16">
         <v>115</v>
@@ -794,15 +794,15 @@
         <v>113</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>115</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17">
         <v>117</v>
@@ -811,99 +811,99 @@
         <v>120</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>116</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18">
         <v>117</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>117</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19">
         <v>118</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>118</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C20">
         <v>119</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>119</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21">
         <v>120</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>120</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22">
         <v>121</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>121</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23">
         <v>122</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>122</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24">
         <v>109</v>
@@ -912,7 +912,7 @@
         <v>112</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>